<commit_message>
update script to create quality suites and checks
</commit_message>
<xml_diff>
--- a/mesh-adoption/quality/bd-quality-suite-check-creation/quality_suite_check/resources/quality-config.xlsx
+++ b/mesh-adoption/quality/bd-quality-suite-check-creation/quality_suite_check/resources/quality-config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://quantyca-my.sharepoint.com/personal/tommaso_vitali_quantyca_it/Documents/Desktop/data-quality-script/quality_suite_check/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="244" documentId="8_{B140EA21-06BA-408C-925C-3AF25BA43B82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6C9D572C-F8D9-47B5-B886-F725C7C26728}"/>
+  <xr:revisionPtr revIDLastSave="248" documentId="8_{B140EA21-06BA-408C-925C-3AF25BA43B82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C9CB9180-978D-4C9B-8F77-AE62F9F530C5}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="1" xr2:uid="{5F329870-B02A-4ABE-9749-58154F59453C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="2" xr2:uid="{5F329870-B02A-4ABE-9749-58154F59453C}"/>
   </bookViews>
   <sheets>
     <sheet name="DIM" sheetId="4" state="hidden" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="45">
   <si>
     <t>Business Domain</t>
   </si>
@@ -171,6 +171,9 @@
   </si>
   <si>
     <t>dit_dicox_dpflab_dds2_dev-ddsdltdb.segnogiornalieroquartoorario-PK-ExpectColumnValuesToNotBeNull</t>
+  </si>
+  <si>
+    <t>Description</t>
   </si>
 </sst>
 </file>
@@ -214,13 +217,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -639,7 +645,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87096108-000B-401F-9367-07E52875FB8F}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -678,18 +684,21 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA46CC94-F1DB-4127-820E-DAB1BD4279DC}">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G9" sqref="G2:G9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="42.85546875" customWidth="1"/>
     <col min="3" max="4" width="21.42578125" customWidth="1"/>
     <col min="5" max="6" width="11.42578125" customWidth="1"/>
+    <col min="7" max="7" width="71.42578125" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
@@ -708,8 +717,11 @@
       <c r="F1" s="2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G1" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -729,7 +741,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>33</v>
       </c>
@@ -749,7 +761,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -769,7 +781,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>33</v>
       </c>
@@ -789,7 +801,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -809,7 +821,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>33</v>
       </c>
@@ -829,7 +841,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -849,7 +861,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>33</v>
       </c>

</xml_diff>